<commit_message>
fex_imputil.m utility for fexc generation
this function adds routines to import csv files produced by the latest
Emotient release. A bug in eviewerhdrs.xlsx (prevents to import
surprise and sadness) was also corrected.
</commit_message>
<xml_diff>
--- a/1.0.1/util/eviewerhdrs.xlsx
+++ b/1.0.1/util/eviewerhdrs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="137">
   <si>
     <t>AU1</t>
   </si>
@@ -409,9 +409,6 @@
   </si>
   <si>
     <t>sentiment</t>
-  </si>
-  <si>
-    <t>emotion</t>
   </si>
   <si>
     <t>emotion_intensity</t>
@@ -1088,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1101,7 +1098,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>124</v>
@@ -1449,7 +1446,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>29</v>
@@ -1460,7 +1457,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>30</v>
@@ -1471,7 +1468,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="11" t="s">
@@ -1480,7 +1477,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="11" t="s">
@@ -1489,7 +1486,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="11" t="s">
@@ -1498,7 +1495,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="11" t="s">
@@ -1507,7 +1504,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="11" t="s">
@@ -1516,7 +1513,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="11" t="s">
@@ -1525,7 +1522,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="11" t="s">
@@ -1534,7 +1531,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="11" t="s">
@@ -1543,7 +1540,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="11" t="s">
@@ -1552,7 +1549,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="11" t="s">
@@ -1561,7 +1558,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="11" t="s">
@@ -1570,7 +1567,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="11" t="s">
@@ -1579,7 +1576,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>70</v>
@@ -1590,7 +1587,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>69</v>
@@ -1601,7 +1598,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>67</v>
@@ -1612,7 +1609,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>68</v>
@@ -1650,7 +1647,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>35</v>
@@ -1661,7 +1658,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>37</v>
@@ -1672,7 +1669,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>39</v>
@@ -1683,7 +1680,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>41</v>
@@ -1694,7 +1691,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>43</v>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>45</v>
@@ -1716,7 +1713,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>47</v>
@@ -1727,7 +1724,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>49</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>51</v>
@@ -1749,7 +1746,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>53</v>
@@ -1760,7 +1757,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>55</v>
@@ -1771,7 +1768,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>57</v>
@@ -1782,7 +1779,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>59</v>
@@ -1793,7 +1790,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>61</v>
@@ -1804,7 +1801,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>71</v>
@@ -1815,7 +1812,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>72</v>
@@ -1826,7 +1823,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>73</v>
@@ -1837,7 +1834,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>74</v>

</xml_diff>